<commit_message>
feat(excel): implement Excel template reading and database insertion
- Add GetExcelFromTemplateXlsxContextResultModel for API response
- Create GetExcelFromTemplateXlsxContextDataModel for service layer
- Implement StoreOrderDto for database operations
- Add IStoreOrderProvider and IDataBaseSettingProvider interfaces
- Implement StoreOrderProvider for database insertion
- Create DataBaseSettingProvider for connection string management
- Configure ServeiceMappingProfile for AutoMapper
- Update ExcelReaderAPIController to read Excel template and process data
- Integrate new components in Program.cs

This commit introduces the functionality to read Excel templates,
process the data, and insert it into the database. It includes
new models, providers, and mapping configurations to support
the feature.
</commit_message>
<xml_diff>
--- a/EXCEL_PDF_Practice_sln/Template/FackData20240907.xlsx
+++ b/EXCEL_PDF_Practice_sln/Template/FackData20240907.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t xml:space="preserve">訂單號碼</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">日期</t>
+  </si>
+  <si>
+    <t xml:space="preserve">數量</t>
   </si>
   <si>
     <t xml:space="preserve">ORD5642</t>
@@ -379,12 +382,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,11 +407,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,373 +534,436 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="6" t="n">
         <v>45389</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="6" t="n">
         <v>45058</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="6" t="n">
         <v>45153</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="6" t="n">
         <v>45125</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="6" t="n">
         <v>45408</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="6" t="n">
         <v>45174</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="6" t="n">
         <v>45444</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="6" t="n">
         <v>45046</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="6" t="n">
         <v>45456</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="6" t="n">
         <v>45087</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="6" t="n">
         <v>45072</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E13" s="6" t="n">
         <v>44963</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
+      <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="6" t="n">
         <v>45151</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>14</v>
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="6" t="n">
         <v>45195</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="6" t="n">
         <v>45446</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="6" t="n">
         <v>45030</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>7</v>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="6" t="n">
         <v>45013</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>19</v>
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="6" t="n">
         <v>45334</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>21</v>
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="6" t="n">
         <v>45262</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="6" t="n">
         <v>45041</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>